<commit_message>
Activity Diagrams and design changes
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\IIT\AIDS Degree Details\Y2S1\CM2601 - Object Orientated Development\Coursework\CW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE1F19D-D3AA-4712-A156-A9F0EC3A75DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F056F0B-145D-4449-8467-4015D617E17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,38 +497,45 @@
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
modifications for use case descriptions and activity diagrams
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\IIT\AIDS Degree Details\Y2S1\CM2601 - Object Orientated Development\Coursework\CW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F056F0B-145D-4449-8467-4015D617E17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6850693F-7766-4F21-BAF9-6A24A1E42008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2120" yWindow="810" windowWidth="13830" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>USE CASE DIAGRAM</t>
   </si>
@@ -64,16 +64,29 @@
   </si>
   <si>
     <t>Database Implementation</t>
+  </si>
+  <si>
+    <t>CLASS DIAGRAM</t>
+  </si>
+  <si>
+    <t>SEQUENCE DIAGRAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -121,6 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -404,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E21"/>
+  <dimension ref="B1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,7 +447,7 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -443,7 +457,7 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -451,7 +465,7 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -459,7 +473,7 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
@@ -467,7 +481,7 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
@@ -475,7 +489,7 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
@@ -483,7 +497,7 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
@@ -498,46 +512,97 @@
         <v>2</v>
       </c>
       <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>12</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -545,5 +610,6 @@
     <mergeCell ref="B4:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>